<commit_message>
EDA identify extreme alarming countries in 2000, observe their evolution, GHI Scores ordered by the most import, comparison extreme alarming countries with their GHI 2022: What can we say ?
</commit_message>
<xml_diff>
--- a/GHI analysis/ghi_2000_2022_final_dataframe.xlsx
+++ b/GHI analysis/ghi_2000_2022_final_dataframe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3757a171cf8daaf/Bureau/GHI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3757a171cf8daaf/Bureau/GHI/GHI analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="11_6231F08EF327E9E656721D24B82CE1954FF03A82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B9C7166-43DB-4A80-8939-7F85168A4C11}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="11_6231F08EF327E9E656721D24B82CE1954FF03A82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBCE0A9C-3495-480F-A865-005472AEE284}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-885" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="2022 GHI scores - Tableau 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2022 GHI Ranking - Tableau 1'!$A$1:$E$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2022 GHI Ranking - Tableau 1'!$A$1:$E$134</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="178">
   <si>
     <t>Country</t>
   </si>
@@ -1008,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1187,7 +1187,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1321,10 +1320,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2402,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K135"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2415,28 +2410,28 @@
     <col min="3" max="3" width="19.6328125" style="88" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" style="88" customWidth="1"/>
     <col min="5" max="5" width="18.453125" style="88" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="102" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" style="101" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="8.81640625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="106" t="s">
         <v>177</v>
       </c>
       <c r="G1" s="3"/>
@@ -2461,7 +2456,7 @@
       <c r="E2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="99">
+      <c r="F2" s="98">
         <v>0</v>
       </c>
       <c r="G2" s="83"/>
@@ -2471,7 +2466,7 @@
       <c r="K2" s="83"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="103" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="75">
@@ -2486,7 +2481,7 @@
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="99">
+      <c r="F3" s="98">
         <v>0</v>
       </c>
       <c r="G3" s="3"/>
@@ -2511,7 +2506,7 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="98">
         <v>0</v>
       </c>
       <c r="G4" s="3"/>
@@ -2536,7 +2531,7 @@
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="98">
         <v>0</v>
       </c>
       <c r="G5" s="3"/>
@@ -2561,7 +2556,7 @@
       <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="99">
+      <c r="F6" s="98">
         <v>0</v>
       </c>
       <c r="G6" s="3"/>
@@ -2586,7 +2581,7 @@
       <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="99">
+      <c r="F7" s="98">
         <v>0</v>
       </c>
       <c r="G7" s="3"/>
@@ -2611,7 +2606,7 @@
       <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="99">
+      <c r="F8" s="98">
         <v>0</v>
       </c>
       <c r="G8" s="3"/>
@@ -2636,7 +2631,7 @@
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="99">
+      <c r="F9" s="98">
         <v>0</v>
       </c>
       <c r="G9" s="3"/>
@@ -2661,7 +2656,7 @@
       <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="98">
         <v>0</v>
       </c>
       <c r="G10" s="3"/>
@@ -2686,7 +2681,7 @@
       <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="99">
+      <c r="F11" s="98">
         <v>0</v>
       </c>
       <c r="G11" s="3"/>
@@ -2711,7 +2706,7 @@
       <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="99">
+      <c r="F12" s="98">
         <v>0</v>
       </c>
       <c r="G12" s="3"/>
@@ -2736,7 +2731,7 @@
       <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="99">
+      <c r="F13" s="98">
         <v>0</v>
       </c>
       <c r="G13" s="3"/>
@@ -2761,7 +2756,7 @@
       <c r="E14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="99">
+      <c r="F14" s="98">
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
@@ -2786,7 +2781,7 @@
       <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="99">
+      <c r="F15" s="98">
         <v>0</v>
       </c>
       <c r="G15" s="3"/>
@@ -2811,7 +2806,7 @@
       <c r="E16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="99">
+      <c r="F16" s="98">
         <v>0</v>
       </c>
       <c r="G16" s="3"/>
@@ -2821,7 +2816,7 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="102" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="75">
@@ -2836,7 +2831,7 @@
       <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="99">
+      <c r="F17" s="98">
         <v>0</v>
       </c>
       <c r="G17" s="3"/>
@@ -2861,7 +2856,7 @@
       <c r="E18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="99">
+      <c r="F18" s="98">
         <v>0</v>
       </c>
       <c r="G18" s="3"/>
@@ -2886,7 +2881,7 @@
       <c r="E19" s="5">
         <v>5.3</v>
       </c>
-      <c r="F19" s="99">
+      <c r="F19" s="98">
         <v>0</v>
       </c>
       <c r="G19" s="3"/>
@@ -2911,7 +2906,7 @@
       <c r="E20" s="87">
         <v>5.3</v>
       </c>
-      <c r="F20" s="99">
+      <c r="F20" s="98">
         <v>0</v>
       </c>
       <c r="G20" s="3"/>
@@ -2936,7 +2931,7 @@
       <c r="E21" s="8">
         <v>5.4</v>
       </c>
-      <c r="F21" s="99">
+      <c r="F21" s="98">
         <v>0</v>
       </c>
       <c r="G21" s="3"/>
@@ -2961,7 +2956,7 @@
       <c r="E22" s="8">
         <v>5.6</v>
       </c>
-      <c r="F22" s="99">
+      <c r="F22" s="98">
         <v>0</v>
       </c>
       <c r="G22" s="3"/>
@@ -2986,7 +2981,7 @@
       <c r="E23" s="8">
         <v>5.7</v>
       </c>
-      <c r="F23" s="99">
+      <c r="F23" s="98">
         <v>0</v>
       </c>
       <c r="G23" s="3"/>
@@ -3011,7 +3006,7 @@
       <c r="E24" s="8">
         <v>5.7</v>
       </c>
-      <c r="F24" s="99">
+      <c r="F24" s="98">
         <v>0</v>
       </c>
       <c r="G24" s="3"/>
@@ -3036,7 +3031,7 @@
       <c r="E25" s="8">
         <v>5.9</v>
       </c>
-      <c r="F25" s="99">
+      <c r="F25" s="98">
         <v>0</v>
       </c>
       <c r="G25" s="3"/>
@@ -3061,7 +3056,7 @@
       <c r="E26" s="87">
         <v>5.9</v>
       </c>
-      <c r="F26" s="99">
+      <c r="F26" s="98">
         <v>0</v>
       </c>
       <c r="G26" s="3"/>
@@ -3086,7 +3081,7 @@
       <c r="E27" s="87">
         <v>6.1</v>
       </c>
-      <c r="F27" s="99">
+      <c r="F27" s="98">
         <v>0</v>
       </c>
       <c r="G27" s="3"/>
@@ -3111,7 +3106,7 @@
       <c r="E28" s="8">
         <v>6.2</v>
       </c>
-      <c r="F28" s="99">
+      <c r="F28" s="98">
         <v>0</v>
       </c>
       <c r="G28" s="3"/>
@@ -3121,7 +3116,7 @@
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="103" t="s">
+      <c r="A29" s="102" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="75">
@@ -3136,7 +3131,7 @@
       <c r="E29" s="8">
         <v>6.4</v>
       </c>
-      <c r="F29" s="99">
+      <c r="F29" s="98">
         <v>0</v>
       </c>
       <c r="G29" s="3"/>
@@ -3146,7 +3141,7 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="103" t="s">
+      <c r="A30" s="102" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="75">
@@ -3161,7 +3156,7 @@
       <c r="E30" s="8">
         <v>6.5</v>
       </c>
-      <c r="F30" s="99">
+      <c r="F30" s="98">
         <v>0</v>
       </c>
       <c r="G30" s="3"/>
@@ -3186,7 +3181,7 @@
       <c r="E31" s="8">
         <v>6.7</v>
       </c>
-      <c r="F31" s="99">
+      <c r="F31" s="98">
         <v>0</v>
       </c>
       <c r="G31" s="3"/>
@@ -3211,7 +3206,7 @@
       <c r="E32" s="8">
         <v>6.8</v>
       </c>
-      <c r="F32" s="99">
+      <c r="F32" s="98">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
@@ -3236,7 +3231,7 @@
       <c r="E33" s="8">
         <v>6.9</v>
       </c>
-      <c r="F33" s="99">
+      <c r="F33" s="98">
         <v>0</v>
       </c>
       <c r="G33" s="3"/>
@@ -3261,7 +3256,7 @@
       <c r="E34" s="8">
         <v>6.9</v>
       </c>
-      <c r="F34" s="99">
+      <c r="F34" s="98">
         <v>0</v>
       </c>
       <c r="G34" s="3"/>
@@ -3286,7 +3281,7 @@
       <c r="E35" s="8">
         <v>6.9</v>
       </c>
-      <c r="F35" s="99">
+      <c r="F35" s="98">
         <v>0</v>
       </c>
       <c r="G35" s="3"/>
@@ -3311,7 +3306,7 @@
       <c r="E36" s="8">
         <v>7</v>
       </c>
-      <c r="F36" s="99">
+      <c r="F36" s="98">
         <v>0</v>
       </c>
       <c r="G36" s="3"/>
@@ -3336,7 +3331,7 @@
       <c r="E37" s="8">
         <v>7.5</v>
       </c>
-      <c r="F37" s="99">
+      <c r="F37" s="98">
         <v>0</v>
       </c>
       <c r="G37" s="3"/>
@@ -3361,7 +3356,7 @@
       <c r="E38" s="8">
         <v>7.5</v>
       </c>
-      <c r="F38" s="99">
+      <c r="F38" s="98">
         <v>0</v>
       </c>
       <c r="G38" s="3"/>
@@ -3386,7 +3381,7 @@
       <c r="E39" s="8">
         <v>7.6</v>
       </c>
-      <c r="F39" s="99">
+      <c r="F39" s="98">
         <v>0</v>
       </c>
       <c r="G39" s="3"/>
@@ -3411,7 +3406,7 @@
       <c r="E40" s="8">
         <v>7.6</v>
       </c>
-      <c r="F40" s="99">
+      <c r="F40" s="98">
         <v>0</v>
       </c>
       <c r="G40" s="3"/>
@@ -3436,7 +3431,7 @@
       <c r="E41" s="8">
         <v>7.8</v>
       </c>
-      <c r="F41" s="99">
+      <c r="F41" s="98">
         <v>0</v>
       </c>
       <c r="G41" s="3"/>
@@ -3461,7 +3456,7 @@
       <c r="E42" s="8">
         <v>8</v>
       </c>
-      <c r="F42" s="99">
+      <c r="F42" s="98">
         <v>0</v>
       </c>
       <c r="G42" s="3"/>
@@ -3486,7 +3481,7 @@
       <c r="E43" s="8">
         <v>8.1</v>
       </c>
-      <c r="F43" s="99">
+      <c r="F43" s="98">
         <v>0</v>
       </c>
       <c r="G43" s="3"/>
@@ -3511,7 +3506,7 @@
       <c r="E44" s="8">
         <v>8.1</v>
       </c>
-      <c r="F44" s="99">
+      <c r="F44" s="98">
         <v>0</v>
       </c>
       <c r="G44" s="3"/>
@@ -3536,7 +3531,7 @@
       <c r="E45" s="8">
         <v>8.4</v>
       </c>
-      <c r="F45" s="99">
+      <c r="F45" s="98">
         <v>0</v>
       </c>
       <c r="G45" s="3"/>
@@ -3561,7 +3556,7 @@
       <c r="E46" s="8">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F46" s="99">
+      <c r="F46" s="98">
         <v>0</v>
       </c>
       <c r="G46" s="3"/>
@@ -3571,7 +3566,7 @@
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="103" t="s">
+      <c r="A47" s="102" t="s">
         <v>51</v>
       </c>
       <c r="B47" s="75">
@@ -3586,7 +3581,7 @@
       <c r="E47" s="8">
         <v>9</v>
       </c>
-      <c r="F47" s="99">
+      <c r="F47" s="98">
         <v>0</v>
       </c>
       <c r="G47" s="3"/>
@@ -3611,7 +3606,7 @@
       <c r="E48" s="8">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F48" s="99">
+      <c r="F48" s="98">
         <v>0</v>
       </c>
       <c r="G48" s="3"/>
@@ -3636,7 +3631,7 @@
       <c r="E49" s="8">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F49" s="99">
+      <c r="F49" s="98">
         <v>0</v>
       </c>
       <c r="G49" s="3"/>
@@ -3661,7 +3656,7 @@
       <c r="E50" s="8">
         <v>9.5</v>
       </c>
-      <c r="F50" s="99">
+      <c r="F50" s="98">
         <v>0</v>
       </c>
       <c r="G50" s="3"/>
@@ -3686,7 +3681,7 @@
       <c r="E51" s="8">
         <v>10.199999999999999</v>
       </c>
-      <c r="F51" s="99">
+      <c r="F51" s="98">
         <v>0</v>
       </c>
       <c r="G51" s="3"/>
@@ -3711,7 +3706,7 @@
       <c r="E52" s="8">
         <v>10.4</v>
       </c>
-      <c r="F52" s="99">
+      <c r="F52" s="98">
         <v>0</v>
       </c>
       <c r="G52" s="3"/>
@@ -3736,7 +3731,7 @@
       <c r="E53" s="8">
         <v>10.5</v>
       </c>
-      <c r="F53" s="99">
+      <c r="F53" s="98">
         <v>0</v>
       </c>
       <c r="G53" s="3"/>
@@ -3761,7 +3756,7 @@
       <c r="E54" s="8">
         <v>10.6</v>
       </c>
-      <c r="F54" s="99">
+      <c r="F54" s="98">
         <v>0</v>
       </c>
       <c r="G54" s="3"/>
@@ -3771,7 +3766,7 @@
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="103" t="s">
+      <c r="A55" s="102" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="75">
@@ -3786,7 +3781,7 @@
       <c r="E55" s="8">
         <v>11.8</v>
       </c>
-      <c r="F55" s="99">
+      <c r="F55" s="98">
         <v>0</v>
       </c>
       <c r="G55" s="3"/>
@@ -3811,7 +3806,7 @@
       <c r="E56" s="8">
         <v>11.9</v>
       </c>
-      <c r="F56" s="99">
+      <c r="F56" s="98">
         <v>0</v>
       </c>
       <c r="G56" s="3"/>
@@ -3836,7 +3831,7 @@
       <c r="E57" s="8">
         <v>12</v>
       </c>
-      <c r="F57" s="99">
+      <c r="F57" s="98">
         <v>0</v>
       </c>
       <c r="G57" s="3"/>
@@ -3861,7 +3856,7 @@
       <c r="E58" s="8">
         <v>12.3</v>
       </c>
-      <c r="F58" s="99">
+      <c r="F58" s="98">
         <v>0</v>
       </c>
       <c r="G58" s="3"/>
@@ -3886,7 +3881,7 @@
       <c r="E59" s="8">
         <v>12.5</v>
       </c>
-      <c r="F59" s="99">
+      <c r="F59" s="98">
         <v>0</v>
       </c>
       <c r="G59" s="3"/>
@@ -3911,7 +3906,7 @@
       <c r="E60" s="8">
         <v>12.9</v>
       </c>
-      <c r="F60" s="99">
+      <c r="F60" s="98">
         <v>0</v>
       </c>
       <c r="G60" s="3"/>
@@ -3936,7 +3931,7 @@
       <c r="E61" s="8">
         <v>13</v>
       </c>
-      <c r="F61" s="99">
+      <c r="F61" s="98">
         <v>0</v>
       </c>
       <c r="G61" s="3"/>
@@ -3946,7 +3941,7 @@
       <c r="K61" s="3"/>
     </row>
     <row r="62" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="103" t="s">
+      <c r="A62" s="102" t="s">
         <v>66</v>
       </c>
       <c r="B62" s="75">
@@ -3961,7 +3956,7 @@
       <c r="E62" s="8">
         <v>13.2</v>
       </c>
-      <c r="F62" s="99">
+      <c r="F62" s="98">
         <v>0</v>
       </c>
       <c r="G62" s="3"/>
@@ -3986,7 +3981,7 @@
       <c r="E63" s="8">
         <v>13.4</v>
       </c>
-      <c r="F63" s="99">
+      <c r="F63" s="98">
         <v>0</v>
       </c>
       <c r="G63" s="3"/>
@@ -4011,7 +4006,7 @@
       <c r="E64" s="8">
         <v>13.4</v>
       </c>
-      <c r="F64" s="99">
+      <c r="F64" s="98">
         <v>0</v>
       </c>
       <c r="G64" s="3"/>
@@ -4036,7 +4031,7 @@
       <c r="E65" s="8">
         <v>13.6</v>
       </c>
-      <c r="F65" s="99">
+      <c r="F65" s="98">
         <v>0</v>
       </c>
       <c r="G65" s="3"/>
@@ -4061,7 +4056,7 @@
       <c r="E66" s="8">
         <v>13.6</v>
       </c>
-      <c r="F66" s="99">
+      <c r="F66" s="98">
         <v>0</v>
       </c>
       <c r="G66" s="3"/>
@@ -4086,7 +4081,7 @@
       <c r="E67" s="8">
         <v>13.7</v>
       </c>
-      <c r="F67" s="99">
+      <c r="F67" s="98">
         <v>0</v>
       </c>
       <c r="G67" s="3"/>
@@ -4111,7 +4106,7 @@
       <c r="E68" s="8">
         <v>13.9</v>
       </c>
-      <c r="F68" s="99">
+      <c r="F68" s="98">
         <v>0</v>
       </c>
       <c r="G68" s="3"/>
@@ -4136,7 +4131,7 @@
       <c r="E69" s="8">
         <v>13.9</v>
       </c>
-      <c r="F69" s="99">
+      <c r="F69" s="98">
         <v>0</v>
       </c>
       <c r="G69" s="3"/>
@@ -4161,7 +4156,7 @@
       <c r="E70" s="8">
         <v>14.8</v>
       </c>
-      <c r="F70" s="99">
+      <c r="F70" s="98">
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
@@ -4186,7 +4181,7 @@
       <c r="E71" s="8">
         <v>15.2</v>
       </c>
-      <c r="F71" s="99">
+      <c r="F71" s="98">
         <v>0</v>
       </c>
       <c r="G71" s="3"/>
@@ -4211,7 +4206,7 @@
       <c r="E72" s="8">
         <v>15.6</v>
       </c>
-      <c r="F72" s="99">
+      <c r="F72" s="98">
         <v>0</v>
       </c>
       <c r="G72" s="3"/>
@@ -4236,7 +4231,7 @@
       <c r="E73" s="8">
         <v>15.6</v>
       </c>
-      <c r="F73" s="99">
+      <c r="F73" s="98">
         <v>0</v>
       </c>
       <c r="G73" s="3"/>
@@ -4261,7 +4256,7 @@
       <c r="E74" s="8">
         <v>16.3</v>
       </c>
-      <c r="F74" s="99">
+      <c r="F74" s="98">
         <v>0</v>
       </c>
       <c r="G74" s="3"/>
@@ -4271,7 +4266,7 @@
       <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="103" t="s">
+      <c r="A75" s="102" t="s">
         <v>79</v>
       </c>
       <c r="B75" s="75">
@@ -4286,7 +4281,7 @@
       <c r="E75" s="8">
         <v>16.8</v>
       </c>
-      <c r="F75" s="99">
+      <c r="F75" s="98">
         <v>0</v>
       </c>
       <c r="G75" s="3"/>
@@ -4311,7 +4306,7 @@
       <c r="E76" s="8">
         <v>17.100000000000001</v>
       </c>
-      <c r="F76" s="99">
+      <c r="F76" s="98">
         <v>0</v>
       </c>
       <c r="G76" s="3"/>
@@ -4336,7 +4331,7 @@
       <c r="E77" s="8">
         <v>17.2</v>
       </c>
-      <c r="F77" s="99">
+      <c r="F77" s="98">
         <v>0</v>
       </c>
       <c r="G77" s="3"/>
@@ -4361,7 +4356,7 @@
       <c r="E78" s="8">
         <v>17.899999999999999</v>
       </c>
-      <c r="F78" s="99">
+      <c r="F78" s="98">
         <v>0</v>
       </c>
       <c r="G78" s="3"/>
@@ -4386,7 +4381,7 @@
       <c r="E79" s="8">
         <v>18.7</v>
       </c>
-      <c r="F79" s="99">
+      <c r="F79" s="98">
         <v>0</v>
       </c>
       <c r="G79" s="3"/>
@@ -4411,7 +4406,7 @@
       <c r="E80" s="8">
         <v>18.8</v>
       </c>
-      <c r="F80" s="99">
+      <c r="F80" s="98">
         <v>0</v>
       </c>
       <c r="G80" s="3"/>
@@ -4436,7 +4431,7 @@
       <c r="E81" s="8">
         <v>18.899999999999999</v>
       </c>
-      <c r="F81" s="99">
+      <c r="F81" s="98">
         <v>0</v>
       </c>
       <c r="G81" s="3"/>
@@ -4461,7 +4456,7 @@
       <c r="E82" s="8">
         <v>19.100000000000001</v>
       </c>
-      <c r="F82" s="99">
+      <c r="F82" s="98">
         <v>0</v>
       </c>
       <c r="G82" s="3"/>
@@ -4471,7 +4466,7 @@
       <c r="K82" s="3"/>
     </row>
     <row r="83" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="103" t="s">
+      <c r="A83" s="102" t="s">
         <v>87</v>
       </c>
       <c r="B83" s="75">
@@ -4486,7 +4481,7 @@
       <c r="E83" s="8">
         <v>19.2</v>
       </c>
-      <c r="F83" s="99">
+      <c r="F83" s="98">
         <v>0</v>
       </c>
       <c r="G83" s="3"/>
@@ -4511,7 +4506,7 @@
       <c r="E84" s="8">
         <v>19.399999999999999</v>
       </c>
-      <c r="F84" s="99">
+      <c r="F84" s="98">
         <v>0</v>
       </c>
       <c r="G84" s="3"/>
@@ -4536,7 +4531,7 @@
       <c r="E85" s="8">
         <v>19.600000000000001</v>
       </c>
-      <c r="F85" s="99">
+      <c r="F85" s="98">
         <v>0</v>
       </c>
       <c r="G85" s="3"/>
@@ -4546,7 +4541,7 @@
       <c r="K85" s="3"/>
     </row>
     <row r="86" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="103" t="s">
+      <c r="A86" s="102" t="s">
         <v>90</v>
       </c>
       <c r="B86" s="75">
@@ -4561,7 +4556,7 @@
       <c r="E86" s="8">
         <v>19.899999999999999</v>
       </c>
-      <c r="F86" s="99">
+      <c r="F86" s="98">
         <v>0</v>
       </c>
       <c r="G86" s="3"/>
@@ -4586,7 +4581,7 @@
       <c r="E87" s="8">
         <v>20</v>
       </c>
-      <c r="F87" s="99">
+      <c r="F87" s="98">
         <v>0</v>
       </c>
       <c r="G87" s="3"/>
@@ -4611,7 +4606,7 @@
       <c r="E88" s="8">
         <v>20.7</v>
       </c>
-      <c r="F88" s="99">
+      <c r="F88" s="98">
         <v>0</v>
       </c>
       <c r="G88" s="3"/>
@@ -4636,7 +4631,7 @@
       <c r="E89" s="8">
         <v>20.7</v>
       </c>
-      <c r="F89" s="99">
+      <c r="F89" s="98">
         <v>0</v>
       </c>
       <c r="G89" s="3"/>
@@ -4661,7 +4656,7 @@
       <c r="E90" s="8">
         <v>20.7</v>
       </c>
-      <c r="F90" s="99">
+      <c r="F90" s="98">
         <v>0</v>
       </c>
       <c r="G90" s="3"/>
@@ -4686,7 +4681,7 @@
       <c r="E91" s="8">
         <v>21.5</v>
       </c>
-      <c r="F91" s="99">
+      <c r="F91" s="98">
         <v>0</v>
       </c>
       <c r="G91" s="3"/>
@@ -4711,7 +4706,7 @@
       <c r="E92" s="8">
         <v>21.7</v>
       </c>
-      <c r="F92" s="99">
+      <c r="F92" s="98">
         <v>0</v>
       </c>
       <c r="G92" s="3"/>
@@ -4736,7 +4731,7 @@
       <c r="E93" s="8">
         <v>22.8</v>
       </c>
-      <c r="F93" s="99">
+      <c r="F93" s="98">
         <v>0</v>
       </c>
       <c r="G93" s="3"/>
@@ -4761,7 +4756,7 @@
       <c r="E94" s="8">
         <v>23.2</v>
       </c>
-      <c r="F94" s="99">
+      <c r="F94" s="98">
         <v>0</v>
       </c>
       <c r="G94" s="3"/>
@@ -4786,7 +4781,7 @@
       <c r="E95" s="8">
         <v>23.5</v>
       </c>
-      <c r="F95" s="99">
+      <c r="F95" s="98">
         <v>0</v>
       </c>
       <c r="G95" s="3"/>
@@ -4796,7 +4791,7 @@
       <c r="K95" s="3"/>
     </row>
     <row r="96" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="103" t="s">
+      <c r="A96" s="102" t="s">
         <v>100</v>
       </c>
       <c r="B96" s="75">
@@ -4811,7 +4806,7 @@
       <c r="E96" s="8">
         <v>23.6</v>
       </c>
-      <c r="F96" s="99">
+      <c r="F96" s="98">
         <v>0</v>
       </c>
       <c r="G96" s="3"/>
@@ -4836,7 +4831,7 @@
       <c r="E97" s="8">
         <v>24.5</v>
       </c>
-      <c r="F97" s="99">
+      <c r="F97" s="98">
         <v>0</v>
       </c>
       <c r="G97" s="3"/>
@@ -4846,7 +4841,7 @@
       <c r="K97" s="3"/>
     </row>
     <row r="98" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="103" t="s">
+      <c r="A98" s="102" t="s">
         <v>102</v>
       </c>
       <c r="B98" s="75">
@@ -4861,7 +4856,7 @@
       <c r="E98" s="8">
         <v>24.9</v>
       </c>
-      <c r="F98" s="99">
+      <c r="F98" s="98">
         <v>0</v>
       </c>
       <c r="G98" s="3"/>
@@ -4886,7 +4881,7 @@
       <c r="E99" s="8">
         <v>25.9</v>
       </c>
-      <c r="F99" s="99">
+      <c r="F99" s="98">
         <v>0</v>
       </c>
       <c r="G99" s="3"/>
@@ -4911,7 +4906,7 @@
       <c r="E100" s="8">
         <v>26.1</v>
       </c>
-      <c r="F100" s="99">
+      <c r="F100" s="98">
         <v>0</v>
       </c>
       <c r="G100" s="3"/>
@@ -4936,7 +4931,7 @@
       <c r="E101" s="8">
         <v>26.5</v>
       </c>
-      <c r="F101" s="99">
+      <c r="F101" s="98">
         <v>0</v>
       </c>
       <c r="G101" s="3"/>
@@ -4961,7 +4956,7 @@
       <c r="E102" s="8">
         <v>26.9</v>
       </c>
-      <c r="F102" s="99">
+      <c r="F102" s="98">
         <v>0</v>
       </c>
       <c r="G102" s="3"/>
@@ -4986,7 +4981,7 @@
       <c r="E103" s="8">
         <v>27.2</v>
       </c>
-      <c r="F103" s="99">
+      <c r="F103" s="98">
         <v>0</v>
       </c>
       <c r="G103" s="3"/>
@@ -5011,7 +5006,7 @@
       <c r="E104" s="8">
         <v>27.3</v>
       </c>
-      <c r="F104" s="99">
+      <c r="F104" s="98">
         <v>0</v>
       </c>
       <c r="G104" s="3"/>
@@ -5036,7 +5031,7 @@
       <c r="E105" s="8">
         <v>27.6</v>
       </c>
-      <c r="F105" s="99">
+      <c r="F105" s="98">
         <v>0</v>
       </c>
       <c r="G105" s="3"/>
@@ -5046,7 +5041,7 @@
       <c r="K105" s="3"/>
     </row>
     <row r="106" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="103" t="s">
+      <c r="A106" s="102" t="s">
         <v>110</v>
       </c>
       <c r="B106" s="75">
@@ -5061,7 +5056,7 @@
       <c r="E106" s="8">
         <v>28.1</v>
       </c>
-      <c r="F106" s="99">
+      <c r="F106" s="98">
         <v>0</v>
       </c>
       <c r="G106" s="3"/>
@@ -5086,7 +5081,7 @@
       <c r="E107" s="8">
         <v>28.8</v>
       </c>
-      <c r="F107" s="99">
+      <c r="F107" s="98">
         <v>0</v>
       </c>
       <c r="G107" s="3"/>
@@ -5111,7 +5106,7 @@
       <c r="E108" s="8">
         <v>29.1</v>
       </c>
-      <c r="F108" s="99">
+      <c r="F108" s="98">
         <v>0</v>
       </c>
       <c r="G108" s="3"/>
@@ -5136,7 +5131,7 @@
       <c r="E109" s="8">
         <v>29.3</v>
       </c>
-      <c r="F109" s="99">
+      <c r="F109" s="98">
         <v>0</v>
       </c>
       <c r="G109" s="3"/>
@@ -5161,7 +5156,7 @@
       <c r="E110" s="8">
         <v>29.9</v>
       </c>
-      <c r="F110" s="99">
+      <c r="F110" s="98">
         <v>0</v>
       </c>
       <c r="G110" s="3"/>
@@ -5186,7 +5181,7 @@
       <c r="E111" s="8">
         <v>30.6</v>
       </c>
-      <c r="F111" s="99">
+      <c r="F111" s="98">
         <v>0</v>
       </c>
       <c r="G111" s="3"/>
@@ -5211,7 +5206,7 @@
       <c r="E112" s="8">
         <v>30.8</v>
       </c>
-      <c r="F112" s="99">
+      <c r="F112" s="98">
         <v>0</v>
       </c>
       <c r="G112" s="3"/>
@@ -5236,7 +5231,7 @@
       <c r="E113" s="8">
         <v>31.5</v>
       </c>
-      <c r="F113" s="99">
+      <c r="F113" s="98">
         <v>0</v>
       </c>
       <c r="G113" s="3"/>
@@ -5261,7 +5256,7 @@
       <c r="E114" s="8">
         <v>32.4</v>
       </c>
-      <c r="F114" s="99">
+      <c r="F114" s="98">
         <v>0</v>
       </c>
       <c r="G114" s="3"/>
@@ -5286,7 +5281,7 @@
       <c r="E115" s="8">
         <v>32.4</v>
       </c>
-      <c r="F115" s="99">
+      <c r="F115" s="98">
         <v>0</v>
       </c>
       <c r="G115" s="6"/>
@@ -5311,7 +5306,7 @@
       <c r="E116" s="8">
         <v>32.6</v>
       </c>
-      <c r="F116" s="99">
+      <c r="F116" s="98">
         <v>0</v>
       </c>
       <c r="G116" s="3"/>
@@ -5336,7 +5331,7 @@
       <c r="E117" s="8">
         <v>32.700000000000003</v>
       </c>
-      <c r="F117" s="99">
+      <c r="F117" s="98">
         <v>0</v>
       </c>
       <c r="G117" s="3"/>
@@ -5361,7 +5356,7 @@
       <c r="E118" s="8">
         <v>27.45</v>
       </c>
-      <c r="F118" s="100">
+      <c r="F118" s="99">
         <v>1</v>
       </c>
       <c r="G118" s="3"/>
@@ -5386,7 +5381,7 @@
       <c r="E119" s="8">
         <v>27.45</v>
       </c>
-      <c r="F119" s="100">
+      <c r="F119" s="99">
         <v>1</v>
       </c>
       <c r="G119" s="3"/>
@@ -5411,7 +5406,7 @@
       <c r="E120" s="8">
         <v>27.45</v>
       </c>
-      <c r="F120" s="100">
+      <c r="F120" s="99">
         <v>1</v>
       </c>
       <c r="G120" s="3"/>
@@ -5436,7 +5431,7 @@
       <c r="E121" s="8">
         <v>27.45</v>
       </c>
-      <c r="F121" s="100">
+      <c r="F121" s="99">
         <v>1</v>
       </c>
       <c r="G121" s="3"/>
@@ -5449,10 +5444,10 @@
       <c r="A122" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="95">
+      <c r="B122" s="94">
         <v>50.7</v>
       </c>
-      <c r="C122" s="95">
+      <c r="C122" s="94">
         <v>49</v>
       </c>
       <c r="D122" s="8">
@@ -5461,7 +5456,7 @@
       <c r="E122" s="8">
         <v>37.200000000000003</v>
       </c>
-      <c r="F122" s="100">
+      <c r="F122" s="99">
         <v>0</v>
       </c>
       <c r="G122" s="3"/>
@@ -5471,13 +5466,13 @@
       <c r="K122" s="3"/>
     </row>
     <row r="123" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="103" t="s">
+      <c r="A123" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="95">
+      <c r="B123" s="94">
         <v>48</v>
       </c>
-      <c r="C123" s="95">
+      <c r="C123" s="94">
         <v>43.2</v>
       </c>
       <c r="D123" s="8">
@@ -5486,7 +5481,7 @@
       <c r="E123" s="8">
         <v>37.799999999999997</v>
       </c>
-      <c r="F123" s="100">
+      <c r="F123" s="99">
         <v>0</v>
       </c>
       <c r="G123" s="3"/>
@@ -5499,10 +5494,10 @@
       <c r="A124" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="95">
+      <c r="B124" s="94">
         <v>42.5</v>
       </c>
-      <c r="C124" s="95">
+      <c r="C124" s="94">
         <v>37.200000000000003</v>
       </c>
       <c r="D124" s="8">
@@ -5511,7 +5506,7 @@
       <c r="E124" s="8">
         <v>38.700000000000003</v>
       </c>
-      <c r="F124" s="100">
+      <c r="F124" s="99">
         <v>0</v>
       </c>
       <c r="G124" s="3"/>
@@ -5521,13 +5516,13 @@
       <c r="K124" s="3"/>
     </row>
     <row r="125" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="103" t="s">
+      <c r="A125" s="102" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="96">
+      <c r="B125" s="95">
         <v>48.8</v>
       </c>
-      <c r="C125" s="96">
+      <c r="C125" s="95">
         <v>46.8</v>
       </c>
       <c r="D125" s="9">
@@ -5536,7 +5531,7 @@
       <c r="E125" s="9">
         <v>37.200000000000003</v>
       </c>
-      <c r="F125" s="100">
+      <c r="F125" s="99">
         <v>0</v>
       </c>
       <c r="G125" s="3"/>
@@ -5546,22 +5541,22 @@
       <c r="K125" s="3"/>
     </row>
     <row r="126" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="91" t="s">
+      <c r="A126" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="97">
+      <c r="B126" s="96">
         <v>41.3</v>
       </c>
-      <c r="C126" s="97">
+      <c r="C126" s="96">
         <v>38.4</v>
       </c>
-      <c r="D126" s="92">
+      <c r="D126" s="91">
         <v>38.700000000000003</v>
       </c>
-      <c r="E126" s="92">
+      <c r="E126" s="91">
         <v>37.799999999999997</v>
       </c>
-      <c r="F126" s="100">
+      <c r="F126" s="99">
         <v>0</v>
       </c>
       <c r="G126" s="2"/>
@@ -5571,22 +5566,22 @@
       <c r="K126" s="3"/>
     </row>
     <row r="127" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="93" t="s">
+      <c r="A127" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="B127" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C127" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D127" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E127" s="92" t="s">
+      <c r="B127" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D127" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="F127" s="101">
+      <c r="F127" s="100">
         <v>1</v>
       </c>
       <c r="G127" s="2"/>
@@ -5596,22 +5591,22 @@
       <c r="K127" s="3"/>
     </row>
     <row r="128" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="93" t="s">
+      <c r="A128" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="B128" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C128" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D128" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E128" s="92" t="s">
+      <c r="B128" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D128" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E128" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="F128" s="101">
+      <c r="F128" s="100">
         <v>1</v>
       </c>
       <c r="G128" s="2"/>
@@ -5621,22 +5616,22 @@
       <c r="K128" s="3"/>
     </row>
     <row r="129" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="93" t="s">
+      <c r="A129" s="92" t="s">
         <v>158</v>
       </c>
-      <c r="B129" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C129" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D129" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E129" s="92" t="s">
+      <c r="B129" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D129" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="F129" s="101">
+      <c r="F129" s="100">
         <v>1</v>
       </c>
       <c r="G129" s="2"/>
@@ -5646,22 +5641,22 @@
       <c r="K129" s="3"/>
     </row>
     <row r="130" spans="1:11" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="93" t="s">
+      <c r="A130" s="92" t="s">
         <v>159</v>
       </c>
-      <c r="B130" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C130" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D130" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E130" s="92" t="s">
+      <c r="B130" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D130" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="F130" s="101">
+      <c r="F130" s="100">
         <v>1</v>
       </c>
       <c r="G130" s="2"/>
@@ -5671,108 +5666,87 @@
       <c r="K130" s="3"/>
     </row>
     <row r="131" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="93" t="s">
-        <v>176</v>
-      </c>
-      <c r="B131" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C131" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D131" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="92" t="s">
-        <v>127</v>
-      </c>
-      <c r="F131" s="101">
+      <c r="A131" s="97" t="s">
+        <v>149</v>
+      </c>
+      <c r="B131" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D131" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F131" s="100">
         <v>1</v>
       </c>
-      <c r="G131" s="90"/>
     </row>
     <row r="132" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="98" t="s">
-        <v>149</v>
-      </c>
-      <c r="B132" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C132" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D132" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E132" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="F132" s="101">
+      <c r="A132" s="97" t="s">
+        <v>152</v>
+      </c>
+      <c r="B132" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E132" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F132" s="100">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="B133" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C133" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D133" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E133" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="F133" s="101">
+      <c r="A133" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B133" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C133" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D133" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E133" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F133" s="100">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="98" t="s">
-        <v>153</v>
-      </c>
-      <c r="B134" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C134" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D134" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E134" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="F134" s="101">
+      <c r="A134" s="97" t="s">
+        <v>156</v>
+      </c>
+      <c r="B134" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C134" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D134" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E134" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F134" s="100">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="98" t="s">
-        <v>156</v>
-      </c>
-      <c r="B135" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C135" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D135" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="E135" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="F135" s="101">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E135" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E134" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -5856,41 +5830,41 @@
     </row>
     <row r="2" spans="1:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="110" t="s">
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
       <c r="N2" s="18"/>
-      <c r="O2" s="110" t="s">
+      <c r="O2" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="110" t="s">
+      <c r="W2" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
+      <c r="X2" s="110"/>
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="110"/>
       <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
       <c r="AC2" s="19"/>
@@ -5905,7 +5879,7 @@
     </row>
     <row r="3" spans="1:37" ht="13.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
-      <c r="B3" s="109"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="21" t="s">
         <v>133</v>
       </c>
@@ -5918,38 +5892,38 @@
       <c r="F3" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="113" t="s">
+      <c r="G3" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="114"/>
-      <c r="I3" s="115" t="s">
+      <c r="H3" s="113"/>
+      <c r="I3" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="114"/>
-      <c r="K3" s="115" t="s">
+      <c r="J3" s="113"/>
+      <c r="K3" s="114" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="114"/>
-      <c r="M3" s="115" t="s">
+      <c r="L3" s="113"/>
+      <c r="M3" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="N3" s="116"/>
-      <c r="O3" s="113" t="s">
+      <c r="N3" s="115"/>
+      <c r="O3" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="115" t="s">
+      <c r="P3" s="113"/>
+      <c r="Q3" s="114" t="s">
         <v>138</v>
       </c>
-      <c r="R3" s="114"/>
-      <c r="S3" s="115" t="s">
+      <c r="R3" s="113"/>
+      <c r="S3" s="114" t="s">
         <v>139</v>
       </c>
-      <c r="T3" s="114"/>
-      <c r="U3" s="115" t="s">
+      <c r="T3" s="113"/>
+      <c r="U3" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="V3" s="116"/>
+      <c r="V3" s="115"/>
       <c r="W3" s="24">
         <v>2000</v>
       </c>

</xml_diff>